<commit_message>
Clackamas/flow2010.ic - Made from Baseline_2010-19_C85plus. Flow.cpp - Elaborate the InitGridIndex() failure message. Turn an ASSERT into a fatal error.
</commit_message>
<xml_diff>
--- a/DataCW3M/SkillAssessment/ClackasmasSummary.xlsx
+++ b/DataCW3M/SkillAssessment/ClackasmasSummary.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CW3M.git\trunk\DataCW3M\CW3MdigitalHandbook\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CW3M.git\trunk\DataCW3M\SkillAssessment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DD05FF8-5C77-4873-AAA6-44B6E8E128EF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{925F7C8B-64BC-4623-80CD-F4CD66A9FE64}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3000" yWindow="240" windowWidth="18852" windowHeight="11328" xr2:uid="{C67948E6-1C73-4AAC-90D2-A2C4D420F2BD}"/>
+    <workbookView xWindow="2304" yWindow="396" windowWidth="20280" windowHeight="10296" xr2:uid="{C67948E6-1C73-4AAC-90D2-A2C4D420F2BD}"/>
   </bookViews>
   <sheets>
     <sheet name="Flow skill" sheetId="3" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="40">
   <si>
     <t>USGS gage</t>
   </si>
@@ -150,6 +150,9 @@
   </si>
   <si>
     <t>CLACKAMAS RIVER AT ESTACADA  OR</t>
+  </si>
+  <si>
+    <t>C85+</t>
   </si>
 </sst>
 </file>
@@ -289,16 +292,11 @@
     <xf numFmtId="2" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -307,7 +305,12 @@
     <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -626,8 +629,8 @@
   <dimension ref="A1:BH14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I14" sqref="I14"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -662,73 +665,73 @@
       <c r="E1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="25" t="s">
+      <c r="I1" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="J1" s="25"/>
-      <c r="K1" s="29" t="s">
+      <c r="J1" s="27"/>
+      <c r="K1" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="L1" s="29"/>
-      <c r="M1" s="30" t="s">
+      <c r="L1" s="28"/>
+      <c r="M1" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="N1" s="30"/>
-      <c r="O1" s="28" t="s">
+      <c r="N1" s="29"/>
+      <c r="O1" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="P1" s="28"/>
-      <c r="Q1" s="25" t="s">
+      <c r="P1" s="30"/>
+      <c r="Q1" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="R1" s="25"/>
+      <c r="R1" s="27"/>
       <c r="S1" s="26" t="s">
         <v>14</v>
       </c>
       <c r="T1" s="26"/>
-      <c r="U1" s="27" t="s">
+      <c r="U1" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="V1" s="27"/>
-      <c r="W1" s="28" t="s">
+      <c r="V1" s="31"/>
+      <c r="W1" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="X1" s="28"/>
+      <c r="X1" s="30"/>
       <c r="Z1" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="AA1" s="25" t="s">
+      <c r="AA1" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="AB1" s="25"/>
-      <c r="AC1" s="29" t="s">
+      <c r="AB1" s="27"/>
+      <c r="AC1" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="AD1" s="29"/>
-      <c r="AE1" s="27" t="s">
+      <c r="AD1" s="28"/>
+      <c r="AE1" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="AF1" s="27"/>
-      <c r="AG1" s="28" t="s">
+      <c r="AF1" s="31"/>
+      <c r="AG1" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="AH1" s="28"/>
-      <c r="AI1" s="25" t="s">
+      <c r="AH1" s="30"/>
+      <c r="AI1" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="AJ1" s="25"/>
+      <c r="AJ1" s="27"/>
       <c r="AK1" s="26" t="s">
         <v>14</v>
       </c>
       <c r="AL1" s="26"/>
-      <c r="AM1" s="27" t="s">
+      <c r="AM1" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="AN1" s="27"/>
-      <c r="AO1" s="28" t="s">
+      <c r="AN1" s="31"/>
+      <c r="AO1" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="AP1" s="28"/>
+      <c r="AP1" s="30"/>
       <c r="AQ1">
         <f>MIN(AQ3:AQ69)</f>
         <v>1</v>
@@ -940,19 +943,19 @@
         <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>10</v>
+        <v>39</v>
       </c>
       <c r="E3" s="3">
-        <v>-0.49</v>
+        <v>0.95</v>
       </c>
       <c r="F3" s="7">
-        <v>-0.52800000000000002</v>
+        <v>-3.1E-2</v>
       </c>
       <c r="G3" s="4">
-        <v>1.22</v>
+        <v>0.221</v>
       </c>
       <c r="H3" s="5">
-        <v>0.86</v>
+        <v>0.95</v>
       </c>
       <c r="I3" s="8">
         <v>0.87517406588218205</v>
@@ -1120,19 +1123,19 @@
         <v>22</v>
       </c>
       <c r="D4" t="s">
-        <v>10</v>
+        <v>39</v>
       </c>
       <c r="E4" s="3">
-        <v>0.39300000000000002</v>
+        <v>0.19800000000000001</v>
       </c>
       <c r="F4" s="7">
-        <v>3.2250000000000001</v>
+        <v>8.4250000000000007</v>
       </c>
       <c r="G4" s="4">
-        <v>0.77800000000000002</v>
+        <v>0.89500000000000002</v>
       </c>
       <c r="H4" s="5">
-        <v>0.73299999999999998</v>
+        <v>0.748</v>
       </c>
       <c r="I4" s="8">
         <v>-6.1650493608395598</v>
@@ -1140,10 +1143,10 @@
       <c r="J4" s="8">
         <v>-6.2054640769481804</v>
       </c>
-      <c r="K4" s="31">
+      <c r="K4" s="25">
         <v>90.817287947932698</v>
       </c>
-      <c r="L4" s="31">
+      <c r="L4" s="25">
         <v>90.677144158421896</v>
       </c>
       <c r="M4" s="9">
@@ -1191,10 +1194,10 @@
       <c r="AB4" s="8">
         <v>-6.0444303011356197</v>
       </c>
-      <c r="AC4" s="31">
+      <c r="AC4" s="25">
         <v>90.992890159462206</v>
       </c>
-      <c r="AD4" s="31">
+      <c r="AD4" s="25">
         <v>90.807583521074704</v>
       </c>
       <c r="AE4" s="9">
@@ -1300,19 +1303,19 @@
         <v>25</v>
       </c>
       <c r="D5" t="s">
-        <v>10</v>
+        <v>39</v>
       </c>
       <c r="E5" s="3">
-        <v>-1.51</v>
+        <v>0.86599999999999999</v>
       </c>
       <c r="F5" s="7">
-        <v>-0.54700000000000004</v>
+        <v>-0.10299999999999999</v>
       </c>
       <c r="G5" s="4">
-        <v>1.5860000000000001</v>
+        <v>0.36499999999999999</v>
       </c>
       <c r="H5" s="5">
-        <v>0.83399999999999996</v>
+        <v>0.91600000000000004</v>
       </c>
       <c r="I5" s="8">
         <v>-0.12579102405015699</v>
@@ -1320,10 +1323,10 @@
       <c r="J5" s="8">
         <v>-0.15731268790108199</v>
       </c>
-      <c r="K5" s="31">
+      <c r="K5" s="25">
         <v>-12.016822324999</v>
       </c>
-      <c r="L5" s="31">
+      <c r="L5" s="25">
         <v>-12.967679592282</v>
       </c>
       <c r="M5" s="9">
@@ -1371,10 +1374,10 @@
       <c r="AB5" s="8">
         <v>-0.112730353061711</v>
       </c>
-      <c r="AC5" s="31">
+      <c r="AC5" s="25">
         <v>-14.713896120325201</v>
       </c>
-      <c r="AD5" s="31">
+      <c r="AD5" s="25">
         <v>-14.186631350404101</v>
       </c>
       <c r="AE5" s="9">
@@ -1480,19 +1483,19 @@
         <v>28</v>
       </c>
       <c r="D6" t="s">
-        <v>10</v>
+        <v>39</v>
       </c>
       <c r="E6" s="3">
-        <v>-96.6</v>
+        <v>-16.73</v>
       </c>
       <c r="F6" s="7">
-        <v>-0.90900000000000003</v>
+        <v>-0.81799999999999995</v>
       </c>
       <c r="G6" s="4">
-        <v>9.8800000000000008</v>
+        <v>4.21</v>
       </c>
       <c r="H6" s="5">
-        <v>0.67800000000000005</v>
+        <v>0.81</v>
       </c>
     </row>
     <row r="7" spans="1:60" x14ac:dyDescent="0.3">
@@ -1506,19 +1509,19 @@
         <v>29</v>
       </c>
       <c r="D7" t="s">
-        <v>10</v>
+        <v>39</v>
       </c>
       <c r="E7" s="3">
-        <v>-0.56100000000000005</v>
+        <v>0.93600000000000005</v>
       </c>
       <c r="F7" s="7">
-        <v>-0.50600000000000001</v>
+        <v>-4.9000000000000002E-2</v>
       </c>
       <c r="G7" s="4">
-        <v>1.2490000000000001</v>
+        <v>0.251</v>
       </c>
       <c r="H7" s="5">
-        <v>0.84599999999999997</v>
+        <v>0.94299999999999995</v>
       </c>
       <c r="I7" s="8">
         <v>0.80940687816865498</v>
@@ -1526,10 +1529,10 @@
       <c r="J7" s="8">
         <v>0.769334859050122</v>
       </c>
-      <c r="K7" s="31">
+      <c r="K7" s="25">
         <v>-4.3526231551944896</v>
       </c>
-      <c r="L7" s="31">
+      <c r="L7" s="25">
         <v>-6.5097568990758301</v>
       </c>
       <c r="M7" s="9">
@@ -1577,10 +1580,10 @@
       <c r="AB7" s="8">
         <v>0.81487431108080899</v>
       </c>
-      <c r="AC7" s="31">
+      <c r="AC7" s="25">
         <v>-8.70200089752535</v>
       </c>
-      <c r="AD7" s="31">
+      <c r="AD7" s="25">
         <v>-7.4905471371135004</v>
       </c>
       <c r="AE7" s="9">
@@ -1686,19 +1689,19 @@
         <v>31</v>
       </c>
       <c r="D8" t="s">
-        <v>10</v>
+        <v>39</v>
       </c>
       <c r="E8" s="3">
-        <v>-0.34</v>
+        <v>0.94699999999999995</v>
       </c>
       <c r="F8" s="7">
-        <v>-0.48199999999999998</v>
+        <v>-8.9999999999999993E-3</v>
       </c>
       <c r="G8" s="4">
-        <v>1.1499999999999999</v>
+        <v>0.22800000000000001</v>
       </c>
       <c r="H8" s="5">
-        <v>0.84599999999999997</v>
+        <v>0.94899999999999995</v>
       </c>
       <c r="I8" s="8">
         <v>0.83191942685365805</v>
@@ -1706,10 +1709,10 @@
       <c r="J8" s="8">
         <v>0.79591027856556695</v>
       </c>
-      <c r="K8" s="31">
+      <c r="K8" s="25">
         <v>0.38831179398619903</v>
       </c>
-      <c r="L8" s="31">
+      <c r="L8" s="25">
         <v>-1.3185495812788199</v>
       </c>
       <c r="M8" s="9">
@@ -1757,10 +1760,10 @@
       <c r="AB8" s="8">
         <v>0.85464863387376999</v>
       </c>
-      <c r="AC8" s="31">
+      <c r="AC8" s="25">
         <v>-3.7988371745056999</v>
       </c>
-      <c r="AD8" s="31">
+      <c r="AD8" s="25">
         <v>-2.1712428863506799</v>
       </c>
       <c r="AE8" s="9">
@@ -1914,19 +1917,19 @@
         <v>37</v>
       </c>
       <c r="D13" t="s">
-        <v>10</v>
+        <v>39</v>
       </c>
       <c r="E13" s="3">
-        <v>0.97899999999999998</v>
+        <v>0.95799999999999996</v>
       </c>
       <c r="F13" s="7">
-        <v>0.03</v>
+        <v>-0.111</v>
       </c>
       <c r="G13" s="4">
-        <v>0.14000000000000001</v>
+        <v>0.20399999999999999</v>
       </c>
       <c r="H13" s="5">
-        <v>0.98</v>
+        <v>0.98099999999999998</v>
       </c>
     </row>
     <row r="14" spans="1:60" x14ac:dyDescent="0.3">
@@ -1957,12 +1960,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="S1:T1"/>
-    <mergeCell ref="I1:J1"/>
-    <mergeCell ref="K1:L1"/>
-    <mergeCell ref="M1:N1"/>
-    <mergeCell ref="O1:P1"/>
-    <mergeCell ref="Q1:R1"/>
     <mergeCell ref="AI1:AJ1"/>
     <mergeCell ref="AK1:AL1"/>
     <mergeCell ref="AM1:AN1"/>
@@ -1973,6 +1970,12 @@
     <mergeCell ref="AC1:AD1"/>
     <mergeCell ref="AE1:AF1"/>
     <mergeCell ref="AG1:AH1"/>
+    <mergeCell ref="S1:T1"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="K1:L1"/>
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="O1:P1"/>
+    <mergeCell ref="Q1:R1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>

</xml_diff>